<commit_message>
Jalama and Cojo Pie Charts finished
</commit_message>
<xml_diff>
--- a/data/Well Lithology.xlsx
+++ b/data/Well Lithology.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="154">
   <si>
     <t>Name</t>
   </si>
@@ -84,7 +84,7 @@
     <t>Brown clay and gravel</t>
   </si>
   <si>
-    <t>clay and gravel</t>
+    <t>clay, gravel</t>
   </si>
   <si>
     <t>Brown claystone</t>
@@ -171,7 +171,7 @@
     <t>Grey siltstone and grey sandstone</t>
   </si>
   <si>
-    <t>siltstone and sandstone</t>
+    <t>siltstone, sandstone</t>
   </si>
   <si>
     <t>Brown sandstone</t>
@@ -183,7 +183,7 @@
     <t>Soil and black clay</t>
   </si>
   <si>
-    <t>soil and clay</t>
+    <t>soil, clay</t>
   </si>
   <si>
     <t>904522</t>
@@ -216,13 +216,13 @@
     <t>Adobe and shale</t>
   </si>
   <si>
-    <t>adobe and shale</t>
+    <t>adobe, shale</t>
   </si>
   <si>
     <t>Shale and clay</t>
   </si>
   <si>
-    <t>shale and clay</t>
+    <t>clay, shale</t>
   </si>
   <si>
     <t>Shale and cemented seashells</t>
@@ -258,7 +258,7 @@
     <t>Sand and gravel</t>
   </si>
   <si>
-    <t>sand and gravel</t>
+    <t>sand, gravel</t>
   </si>
   <si>
     <t>Green sandy shale</t>
@@ -267,7 +267,7 @@
     <t>Green sandy shale with sandstone layers</t>
   </si>
   <si>
-    <t>shale and sandstone</t>
+    <t>shale, sandstone</t>
   </si>
   <si>
     <t>Shale with sandstone layers</t>
@@ -336,7 +336,7 @@
     <t>Shale, gravel, and clay</t>
   </si>
   <si>
-    <t>shale, gravel, and clay</t>
+    <t>shale, gravel, clay</t>
   </si>
   <si>
     <t>e0095907</t>
@@ -354,9 +354,6 @@
     <t>Clay and shale</t>
   </si>
   <si>
-    <t>clay and shale</t>
-  </si>
-  <si>
     <t>Escondido Well #5</t>
   </si>
   <si>
@@ -426,6 +423,9 @@
     <t>Shale, sand, and clay</t>
   </si>
   <si>
+    <t>Shale, sand, clay</t>
+  </si>
+  <si>
     <t>e0098248</t>
   </si>
   <si>
@@ -438,10 +438,16 @@
     <t>Clay, gravel, and sand</t>
   </si>
   <si>
+    <t>Clay, gravel, sand</t>
+  </si>
+  <si>
     <t>Oaks Well #5</t>
   </si>
   <si>
     <t>E070248</t>
+  </si>
+  <si>
+    <t>Shale, gravel, clay</t>
   </si>
   <si>
     <t>Casing from</t>
@@ -2751,7 +2757,7 @@
         <v>105</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>94</v>
@@ -2791,7 +2797,7 @@
         <v>10</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C77" s="1">
         <v>0.0</v>
@@ -2809,7 +2815,7 @@
         <v>94</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="78">
@@ -2817,7 +2823,7 @@
         <v>10</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C78" s="1">
         <v>3.0</v>
@@ -2835,7 +2841,7 @@
         <v>94</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="79">
@@ -2843,7 +2849,7 @@
         <v>10</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C79" s="1">
         <v>9.0</v>
@@ -2852,16 +2858,16 @@
         <v>14.0</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>94</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="80">
@@ -2869,7 +2875,7 @@
         <v>10</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C80" s="1">
         <v>14.0</v>
@@ -2878,7 +2884,7 @@
         <v>22.0</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>25</v>
@@ -2887,7 +2893,7 @@
         <v>94</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="81">
@@ -2895,7 +2901,7 @@
         <v>10</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C81" s="1">
         <v>22.0</v>
@@ -2913,7 +2919,7 @@
         <v>94</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="82">
@@ -2921,7 +2927,7 @@
         <v>10</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C82" s="1">
         <v>29.0</v>
@@ -2939,7 +2945,7 @@
         <v>94</v>
       </c>
       <c r="H82" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83">
@@ -2947,7 +2953,7 @@
         <v>22</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C83" s="1">
         <v>0.0</v>
@@ -2962,10 +2968,10 @@
         <v>43</v>
       </c>
       <c r="G83" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H83" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="84">
@@ -2973,7 +2979,7 @@
         <v>22</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C84" s="1">
         <v>8.0</v>
@@ -2988,10 +2994,10 @@
         <v>25</v>
       </c>
       <c r="G84" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H84" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="H84" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="85">
@@ -2999,7 +3005,7 @@
         <v>22</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C85" s="1">
         <v>55.0</v>
@@ -3008,16 +3014,16 @@
         <v>102.0</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G85" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H85" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="86">
@@ -3025,7 +3031,7 @@
         <v>22</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C86" s="1">
         <v>102.0</v>
@@ -3034,24 +3040,24 @@
         <v>485.0</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G86" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H86" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="C87" s="1">
         <v>45.0</v>
@@ -3060,24 +3066,24 @@
         <v>60.0</v>
       </c>
       <c r="E87" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F87" s="1" t="s">
+      <c r="G87" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G87" s="1" t="s">
+      <c r="H87" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="H87" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="C88" s="1">
         <v>60.0</v>
@@ -3092,18 +3098,18 @@
         <v>25</v>
       </c>
       <c r="G88" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H88" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="H88" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="C89" s="1">
         <v>100.0</v>
@@ -3112,24 +3118,24 @@
         <v>220.0</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G89" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H89" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="H89" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="C90" s="1">
         <v>220.0</v>
@@ -3141,21 +3147,21 @@
         <v>105</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="G90" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H90" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="H90" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C91" s="1">
         <v>0.0</v>
@@ -3170,18 +3176,18 @@
         <v>29</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C92" s="1">
         <v>4.0</v>
@@ -3196,18 +3202,18 @@
         <v>25</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C93" s="1">
         <v>360.0</v>
@@ -3216,24 +3222,24 @@
         <v>363.0</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C94" s="1">
         <v>363.0</v>
@@ -3248,18 +3254,18 @@
         <v>25</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C95" s="1">
         <v>0.0</v>
@@ -3274,18 +3280,18 @@
         <v>100</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C96" s="1">
         <v>35.0</v>
@@ -3300,18 +3306,18 @@
         <v>25</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C97" s="1">
         <v>0.0</v>
@@ -3320,13 +3326,13 @@
         <v>60.0</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>129</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H97" s="2" t="s">
         <v>130</v>
@@ -3334,10 +3340,10 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C98" s="1">
         <v>60.0</v>
@@ -3352,7 +3358,7 @@
         <v>20</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H98" s="2" t="s">
         <v>130</v>
@@ -3360,7 +3366,7 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>131</v>
@@ -3378,7 +3384,7 @@
         <v>12</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H99" s="2" t="s">
         <v>132</v>
@@ -3386,7 +3392,7 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>131</v>
@@ -3401,10 +3407,10 @@
         <v>133</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H100" s="2" t="s">
         <v>132</v>
@@ -3412,7 +3418,7 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>131</v>
@@ -3430,7 +3436,7 @@
         <v>20</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H101" s="2" t="s">
         <v>132</v>
@@ -3438,7 +3444,7 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>131</v>
@@ -3450,13 +3456,13 @@
         <v>99.0</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H102" s="2" t="s">
         <v>132</v>
@@ -3464,7 +3470,7 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>131</v>
@@ -3482,7 +3488,7 @@
         <v>20</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H103" s="2" t="s">
         <v>132</v>
@@ -3490,10 +3496,10 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C104" s="1">
         <v>0.0</v>
@@ -3508,18 +3514,18 @@
         <v>12</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C105" s="1">
         <v>3.0</v>
@@ -3534,18 +3540,18 @@
         <v>20</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C106" s="1">
         <v>18.0</v>
@@ -3557,21 +3563,21 @@
         <v>99</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C107" s="1">
         <v>46.0</v>
@@ -3586,10 +3592,10 @@
         <v>20</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="108">
@@ -6295,22 +6301,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -6342,10 +6348,10 @@
         <v>200.0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>14</v>
@@ -6371,10 +6377,10 @@
         <v>165.0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>26</v>
@@ -6403,10 +6409,10 @@
         <v>300.0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>30</v>
@@ -6435,10 +6441,10 @@
         <v>520.0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>32</v>
@@ -6467,10 +6473,10 @@
         <v>580.0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>37</v>
@@ -6499,10 +6505,10 @@
         <v>800.0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>41</v>
@@ -6528,13 +6534,13 @@
         <v>350.0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9">
@@ -6557,13 +6563,13 @@
         <v>350.0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10">
@@ -6586,10 +6592,10 @@
         <v>405.0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>53</v>
@@ -6597,7 +6603,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B11" s="1">
         <v>0.0</v>
@@ -6615,7 +6621,7 @@
         <v>425.0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>55</v>
@@ -6626,7 +6632,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B12" s="1">
         <v>81.0</v>
@@ -6644,7 +6650,7 @@
         <v>425.0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>55</v>
@@ -6655,7 +6661,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B13" s="1">
         <v>0.0</v>
@@ -6673,7 +6679,7 @@
         <v>524.0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>55</v>
@@ -6702,7 +6708,7 @@
         <v>324.0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>67</v>
@@ -6731,7 +6737,7 @@
         <v>324.0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>67</v>
@@ -6742,7 +6748,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B16" s="1">
         <v>0.0</v>
@@ -6760,7 +6766,7 @@
         <v>600.0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>67</v>
@@ -6771,7 +6777,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B17" s="1">
         <v>0.0</v>
@@ -6789,7 +6795,7 @@
         <v>600.0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>67</v>
@@ -6818,7 +6824,7 @@
         <v>523.0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>67</v>
@@ -6838,7 +6844,7 @@
         <v>523.0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E19" s="1">
         <v>75.0</v>
@@ -6847,7 +6853,7 @@
         <v>523.0</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>67</v>
@@ -6876,7 +6882,7 @@
         <v>320.0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>85</v>
@@ -6905,7 +6911,7 @@
         <v>320.0</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>85</v>
@@ -6934,7 +6940,7 @@
         <v>283.0</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>94</v>
@@ -6963,7 +6969,7 @@
         <v>283.0</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>94</v>
@@ -6992,7 +6998,7 @@
         <v>450.0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>94</v>
@@ -7021,7 +7027,7 @@
         <v>401.0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>94</v>
@@ -7050,7 +7056,7 @@
         <v>401.0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>94</v>
@@ -7079,7 +7085,7 @@
         <v>400.0</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>94</v>
@@ -7108,7 +7114,7 @@
         <v>400.0</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>94</v>
@@ -7119,7 +7125,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B29" s="1">
         <v>0.0</v>
@@ -7137,18 +7143,18 @@
         <v>340.0</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>94</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B30" s="1">
         <v>0.0</v>
@@ -7166,18 +7172,18 @@
         <v>340.0</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>94</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B31" s="1">
         <v>0.0</v>
@@ -7186,7 +7192,7 @@
         <v>480.0</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E31" s="1">
         <v>48.0</v>
@@ -7195,18 +7201,18 @@
         <v>485.0</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B32" s="1">
         <v>0.0</v>
@@ -7224,18 +7230,18 @@
         <v>260.0</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H32" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I32" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B33" s="1">
         <v>0.0</v>
@@ -7253,18 +7259,18 @@
         <v>380.0</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B34" s="1">
         <v>0.0</v>
@@ -7282,18 +7288,18 @@
         <v>380.0</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35" s="1">
         <v>0.0</v>
@@ -7311,18 +7317,18 @@
         <v>305.0</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B36" s="1">
         <v>0.0</v>
@@ -7340,10 +7346,10 @@
         <v>305.0</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>130</v>
@@ -7351,7 +7357,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B37" s="1">
         <v>0.0</v>
@@ -7369,10 +7375,10 @@
         <v>305.0</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>130</v>
@@ -7398,10 +7404,10 @@
         <v>370.0</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>132</v>
@@ -7427,10 +7433,10 @@
         <v>370.0</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>132</v>
@@ -7438,7 +7444,7 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B40" s="1">
         <v>0.0</v>
@@ -7456,18 +7462,18 @@
         <v>280.0</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B41" s="1">
         <v>0.0</v>
@@ -7485,13 +7491,13 @@
         <v>280.0</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42">

</xml_diff>